<commit_message>
Rewrite excel bulk spec parser to fix header errors
Now reports a missing header correctly rather than reporting it as a duplicated
header. Some other error messages are more specific about the row and the
exact error as well.
</commit_message>
<xml_diff>
--- a/tests/import_specifications/test_data/testtabs3full2nodata1empty.xlsx
+++ b/tests/import_specifications/test_data/testtabs3full2nodata1empty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tab1" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,8 @@
     <sheet name="no_data1" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="no_data2" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="empty_tab" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Only 1 row - should be ignored" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Only 2 rows - should be ignored" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,34 +27,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Data type: type1; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Columns: 3; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Version: 1</t>
-    </r>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="57">
+  <si>
+    <t xml:space="preserve">Data type: type1; Columns: 3; Version: 1</t>
   </si>
   <si>
     <t xml:space="preserve">header1</t>
@@ -88,40 +65,12 @@
     <t xml:space="preserve">    </t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Data type: type2; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Columns: 3; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Version: 1</t>
-    </r>
+    <t xml:space="preserve">Data type: type2; Columns: 3; Version: 1</t>
   </si>
   <si>
     <t xml:space="preserve">h1</t>
   </si>
   <si>
-    <t xml:space="preserve">h2</t>
-  </si>
-  <si>
     <t xml:space="preserve">h3</t>
   </si>
   <si>
@@ -131,32 +80,7 @@
     <t xml:space="preserve">super</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Data type: type3; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Columns: 2; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Version: 1</t>
-    </r>
+    <t xml:space="preserve">Data type: type3; Columns: 2; Version: 1</t>
   </si>
   <si>
     <t xml:space="preserve">head1</t>
@@ -168,32 +92,7 @@
     <t xml:space="preserve">some data</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Data type: nodata1; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Columns: 7; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Version: 1</t>
-    </r>
+    <t xml:space="preserve">Data type: nodata1; Columns: 7; Version: 1</t>
   </si>
   <si>
     <t xml:space="preserve">fasta_file</t>
@@ -238,32 +137,7 @@
     <t xml:space="preserve">Spoof Genes for parentless CDS</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Data type: nodata2; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Columns: 7; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Version: 1</t>
-    </r>
+    <t xml:space="preserve">Data type: nodata2; Columns: 7; Version: 1</t>
   </si>
   <si>
     <t xml:space="preserve">sra_staging_file_name</t>
@@ -306,6 +180,24 @@
   </si>
   <si>
     <t xml:space="preserve">Mean Insert Size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foo bar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some </t>
+  </si>
+  <si>
+    <t xml:space="preserve">other </t>
+  </si>
+  <si>
+    <t xml:space="preserve">importer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">something</t>
   </si>
 </sst>
 </file>
@@ -315,7 +207,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -336,11 +228,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -407,10 +294,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -468,22 +355,22 @@
         <v>8.9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>3.4</v>
-      </c>
-    </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C8" s="0" t="s">
         <v>11</v>
       </c>
     </row>
@@ -505,8 +392,8 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -515,20 +402,20 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,13 +431,13 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>42</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -583,15 +470,15 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -604,7 +491,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>1</v>
@@ -640,53 +527,53 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -719,53 +606,53 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="G2" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -786,7 +673,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -804,4 +691,85 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>